<commit_message>
Stats intéressantes, fermer bot quand finit
</commit_message>
<xml_diff>
--- a/output/missingItems.xlsx
+++ b/output/missingItems.xlsx
@@ -433,10 +433,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -445,8 +445,11 @@
     <col width="47" customWidth="1" style="1" min="2" max="2"/>
     <col width="25.140625" customWidth="1" style="1" min="3" max="3"/>
     <col width="17.140625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="1" min="5" max="8"/>
-    <col width="9.140625" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
+    <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -468,6 +471,16 @@
       <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Jours consécutifs</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Next day to save</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -483,10 +496,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -495,8 +508,11 @@
     <col width="47" customWidth="1" style="1" min="2" max="2"/>
     <col width="25.140625" customWidth="1" style="1" min="3" max="3"/>
     <col width="17.140625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="1" min="5" max="8"/>
-    <col width="9.140625" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
+    <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -518,6 +534,16 @@
       <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Jours consécutifs</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Next day to save</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -532,10 +558,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -544,8 +570,11 @@
     <col width="47" customWidth="1" style="1" min="2" max="2"/>
     <col width="25.140625" customWidth="1" style="1" min="3" max="3"/>
     <col width="17.140625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="1" min="5" max="8"/>
-    <col width="9.140625" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
+    <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -567,6 +596,16 @@
       <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Jours consécutifs</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Next day to save</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -581,10 +620,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -593,8 +632,11 @@
     <col width="47" customWidth="1" style="1" min="2" max="2"/>
     <col width="25.140625" customWidth="1" style="1" min="3" max="3"/>
     <col width="17.140625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="1" min="5" max="8"/>
-    <col width="9.140625" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
+    <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -616,6 +658,16 @@
       <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Jours consécutifs</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Next day to save</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -630,10 +682,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -642,8 +694,11 @@
     <col width="47" customWidth="1" style="1" min="2" max="2"/>
     <col width="25.140625" customWidth="1" style="1" min="3" max="3"/>
     <col width="17.140625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="1" min="5" max="8"/>
-    <col width="9.140625" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
+    <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -665,6 +720,16 @@
       <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Jours consécutifs</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Next day to save</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -679,10 +744,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -691,8 +756,11 @@
     <col width="47" customWidth="1" style="1" min="2" max="2"/>
     <col width="25.140625" customWidth="1" style="1" min="3" max="3"/>
     <col width="17.140625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="1" min="5" max="8"/>
-    <col width="9.140625" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
+    <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -714,6 +782,16 @@
       <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Jours consécutifs</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Next day to save</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -728,10 +806,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -740,8 +818,11 @@
     <col width="47" customWidth="1" style="1" min="2" max="2"/>
     <col width="25.140625" customWidth="1" style="1" min="3" max="3"/>
     <col width="17.140625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="1" min="5" max="8"/>
-    <col width="9.140625" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
+    <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -763,6 +844,16 @@
       <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Jours consécutifs</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Next day to save</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -777,10 +868,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -789,8 +880,11 @@
     <col width="47" customWidth="1" style="1" min="2" max="2"/>
     <col width="25.140625" customWidth="1" style="1" min="3" max="3"/>
     <col width="17.140625" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="1" min="5" max="8"/>
-    <col width="9.140625" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
+    <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -814,8 +908,19 @@
           <t>Jours consécutifs</t>
         </is>
       </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Next day to save</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>06-05-2021</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removing consecutive day requirement
</commit_message>
<xml_diff>
--- a/output/missingItems.xlsx
+++ b/output/missingItems.xlsx
@@ -451,8 +451,8 @@
     <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
     <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
     <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="9.140625" customWidth="1" style="1" min="10" max="14"/>
-    <col width="9.140625" customWidth="1" style="1" min="15" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="16"/>
+    <col width="9.140625" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -478,12 +478,12 @@
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Next day to save</t>
+          <t>Last save</t>
         </is>
       </c>
       <c r="I1" s="3" t="inlineStr">
         <is>
-          <t>07-05-2021</t>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -516,7 +516,7 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -530,7 +530,7 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -544,7 +544,7 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -558,7 +558,7 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -572,7 +572,7 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -586,7 +586,7 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -600,7 +600,7 @@
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -614,7 +614,7 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -628,7 +628,7 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -642,7 +642,7 @@
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -656,7 +656,7 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -670,7 +670,7 @@
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -698,7 +698,7 @@
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -712,7 +712,7 @@
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -748,7 +748,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -762,7 +762,7 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -776,7 +776,7 @@
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -806,8 +806,8 @@
     <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
     <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
     <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="9.140625" customWidth="1" style="1" min="10" max="14"/>
-    <col width="9.140625" customWidth="1" style="1" min="15" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="16"/>
+    <col width="9.140625" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -833,12 +833,12 @@
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Next day to save</t>
+          <t>Last save</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>07-05-2021</t>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -867,7 +867,7 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -881,7 +881,7 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -895,7 +895,7 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -913,7 +913,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -927,7 +927,7 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -941,7 +941,7 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -973,7 +973,7 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -987,7 +987,7 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1005,7 +1005,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1023,7 +1023,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1041,7 +1041,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1059,7 +1059,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1091,7 +1091,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1109,7 +1109,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1194,8 +1194,8 @@
     <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
     <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
     <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="9.140625" customWidth="1" style="1" min="10" max="14"/>
-    <col width="9.140625" customWidth="1" style="1" min="15" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="16"/>
+    <col width="9.140625" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1221,12 +1221,12 @@
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Next day to save</t>
+          <t>Last save</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>07-05-2021</t>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1461,7 +1461,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1479,7 +1479,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1535,7 +1535,7 @@
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1581,7 +1581,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1599,7 +1599,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
@@ -1660,8 +1660,8 @@
     <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
     <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
     <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="9.140625" customWidth="1" style="1" min="10" max="14"/>
-    <col width="9.140625" customWidth="1" style="1" min="15" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="16"/>
+    <col width="9.140625" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1687,12 +1687,12 @@
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Next day to save</t>
+          <t>Last save</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>07-05-2021</t>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1739,7 +1739,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1795,7 +1795,7 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1851,21 +1851,25 @@
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Anneau de la mort</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
+          <t>Gantelet du Real Boitar</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>PO</t>
+        </is>
+      </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1874,7 +1878,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Gantelet du Real Boitar</t>
+          <t>Gantelet des Bouftons Rouges</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1883,173 +1887,155 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Gantelet des Bouftons Rouges</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>PO</t>
-        </is>
-      </c>
+          <t>Anneau de Laikteur</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Anneau de Laikteur</t>
+          <t>Anneau de Grizou</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Anneau de Grizou</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
+          <t>Anneau d'Hectaupe</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Invoc</t>
+        </is>
+      </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Anneau d'Hectaupe</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Invoc</t>
-        </is>
-      </c>
+          <t>Anneau Pomdeupin</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Anneau Pomdeupin</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
+          <t>Anneau du Boostache</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Retrait PM</t>
+        </is>
+      </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Anneau du Boostache</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Retrait PM</t>
-        </is>
-      </c>
+          <t>Bracelet du Glutin</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Bracelet du Glutin</t>
+          <t>Bague Rafe</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>43</v>
+        <v>150</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Bague Rafe</t>
+          <t>Mandrano</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>150</v>
+        <v>32</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Mandrano</t>
+          <t>Gant de Frakacia</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Gant de Frakacia</t>
+          <t>Rondelle de Waddict</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>56</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Rondelle de Waddict</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2078,8 +2064,8 @@
     <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
     <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
     <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="9.140625" customWidth="1" style="1" min="10" max="14"/>
-    <col width="9.140625" customWidth="1" style="1" min="15" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="16"/>
+    <col width="9.140625" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2105,12 +2091,12 @@
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Next day to save</t>
+          <t>Last save</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>07-05-2021</t>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -2125,7 +2111,7 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2139,7 +2125,7 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2157,7 +2143,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2171,7 +2157,7 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2189,7 +2175,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2203,7 +2189,7 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2217,7 +2203,7 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2231,7 +2217,7 @@
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2245,7 +2231,7 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2259,7 +2245,7 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2273,7 +2259,7 @@
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2287,7 +2273,7 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2301,7 +2287,7 @@
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -2319,7 +2305,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -2333,7 +2319,7 @@
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -2347,7 +2333,7 @@
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2361,7 +2347,7 @@
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -2375,7 +2361,7 @@
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -2389,7 +2375,7 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -2403,7 +2389,7 @@
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2417,7 +2403,7 @@
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2431,7 +2417,7 @@
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -2445,7 +2431,7 @@
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -2463,7 +2449,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -2481,7 +2467,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -2495,7 +2481,7 @@
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -2513,7 +2499,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -2531,7 +2517,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -2549,7 +2535,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -2567,7 +2553,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -2581,7 +2567,7 @@
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2610,8 +2596,8 @@
     <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
     <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
     <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="9.140625" customWidth="1" style="1" min="10" max="14"/>
-    <col width="9.140625" customWidth="1" style="1" min="15" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="16"/>
+    <col width="9.140625" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2637,12 +2623,12 @@
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Next day to save</t>
+          <t>Last save</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>07-05-2021</t>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -2657,7 +2643,7 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2671,7 +2657,7 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2685,7 +2671,7 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2699,7 +2685,7 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2717,7 +2703,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2731,7 +2717,7 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2745,7 +2731,7 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2763,7 +2749,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2781,7 +2767,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2795,7 +2781,7 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2809,7 +2795,7 @@
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2823,7 +2809,7 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2837,7 +2823,7 @@
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -2855,7 +2841,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -2869,7 +2855,7 @@
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -2887,7 +2873,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2905,7 +2891,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -2923,7 +2909,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -2941,7 +2927,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -2955,7 +2941,7 @@
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2973,7 +2959,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -2987,7 +2973,7 @@
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -3005,7 +2991,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -3023,7 +3009,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -3041,7 +3027,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -3055,7 +3041,7 @@
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -3073,7 +3059,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -3091,7 +3077,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -3105,7 +3091,7 @@
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -3119,7 +3105,7 @@
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -3137,7 +3123,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -3155,7 +3141,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -3169,7 +3155,7 @@
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -3183,7 +3169,7 @@
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -3201,7 +3187,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3230,8 +3216,8 @@
     <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
     <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
     <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="9.140625" customWidth="1" style="1" min="10" max="14"/>
-    <col width="9.140625" customWidth="1" style="1" min="15" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="16"/>
+    <col width="9.140625" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -3257,12 +3243,12 @@
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Next day to save</t>
+          <t>Last save</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>07-05-2021</t>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -3277,7 +3263,7 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -3291,7 +3277,7 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -3305,7 +3291,7 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -3319,7 +3305,7 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -3337,7 +3323,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -3355,7 +3341,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -3369,7 +3355,7 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -3387,7 +3373,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -3401,7 +3387,7 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -3419,7 +3405,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -3437,7 +3423,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -3451,7 +3437,7 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -3465,7 +3451,7 @@
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -3483,7 +3469,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -3501,7 +3487,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -3519,7 +3505,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -3533,7 +3519,7 @@
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -3547,7 +3533,7 @@
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -3561,7 +3547,7 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -3579,7 +3565,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -3593,7 +3579,7 @@
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -3607,7 +3593,7 @@
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -3625,7 +3611,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -3639,7 +3625,7 @@
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -3657,7 +3643,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -3671,7 +3657,7 @@
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -3685,7 +3671,7 @@
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -3703,7 +3689,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -3717,7 +3703,7 @@
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -3735,7 +3721,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -3749,7 +3735,7 @@
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -3763,7 +3749,7 @@
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -3777,7 +3763,7 @@
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -3791,7 +3777,7 @@
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -3805,7 +3791,7 @@
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -3819,7 +3805,7 @@
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -3833,7 +3819,7 @@
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -3851,7 +3837,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -3865,7 +3851,7 @@
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -3879,7 +3865,7 @@
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -3893,7 +3879,7 @@
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -3907,7 +3893,7 @@
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -3921,7 +3907,7 @@
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -3935,7 +3921,7 @@
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -3949,7 +3935,7 @@
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -3963,7 +3949,7 @@
       </c>
       <c r="C47" t="inlineStr"/>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -3977,7 +3963,7 @@
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -3991,7 +3977,7 @@
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -4009,7 +3995,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -4027,7 +4013,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -4041,7 +4027,7 @@
       </c>
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -4055,7 +4041,7 @@
       </c>
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -4069,7 +4055,7 @@
       </c>
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -4083,7 +4069,7 @@
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -4097,7 +4083,7 @@
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -4111,7 +4097,7 @@
       </c>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -4125,7 +4111,7 @@
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -4139,7 +4125,7 @@
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -4153,7 +4139,7 @@
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -4167,7 +4153,7 @@
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -4181,7 +4167,7 @@
       </c>
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -4195,7 +4181,7 @@
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -4213,7 +4199,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -4231,7 +4217,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -4245,7 +4231,7 @@
       </c>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -4259,7 +4245,7 @@
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -4273,7 +4259,7 @@
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -4287,7 +4273,7 @@
       </c>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -4305,7 +4291,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -4319,7 +4305,7 @@
       </c>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -4333,7 +4319,7 @@
       </c>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -4347,7 +4333,7 @@
       </c>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -4361,7 +4347,7 @@
       </c>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -4375,7 +4361,7 @@
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -4389,7 +4375,7 @@
       </c>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4406,7 +4392,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4418,8 +4404,8 @@
     <col width="9.140625" customWidth="1" style="1" min="5" max="7"/>
     <col width="20.140625" customWidth="1" style="1" min="8" max="8"/>
     <col width="13.140625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="9.140625" customWidth="1" style="1" min="10" max="14"/>
-    <col width="9.140625" customWidth="1" style="1" min="15" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="16"/>
+    <col width="9.140625" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -4445,12 +4431,12 @@
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>Next day to save</t>
+          <t>Last save</t>
         </is>
       </c>
       <c r="I1" s="3" t="inlineStr">
         <is>
-          <t>07-05-2021</t>
+          <t>06-05-2021</t>
         </is>
       </c>
     </row>
@@ -4465,7 +4451,7 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -4479,7 +4465,7 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -4493,7 +4479,7 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>